<commit_message>
Thêm xuất excel và update từng dòng
</commit_message>
<xml_diff>
--- a/Template/example_import_capnhatsolieu.xlsx
+++ b/Template/example_import_capnhatsolieu.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cilse\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temp\TAS\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>BẢNG THEO DÕI MỦ FSC BĂNG TÂM</t>
   </si>
@@ -96,14 +96,32 @@
   </si>
   <si>
     <t>NV_3</t>
+  </si>
+  <si>
+    <t>NV_4</t>
+  </si>
+  <si>
+    <t>NV_5</t>
+  </si>
+  <si>
+    <t>NV_6</t>
+  </si>
+  <si>
+    <t>NV_7</t>
+  </si>
+  <si>
+    <t>NV_8</t>
+  </si>
+  <si>
+    <t>NV_9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -220,7 +238,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -238,7 +256,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -248,7 +266,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -257,20 +275,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -557,7 +575,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,7 +680,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>11</v>
@@ -691,7 +709,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>12</v>
@@ -720,7 +738,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>13</v>
@@ -749,7 +767,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>14</v>
@@ -778,7 +796,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>15</v>
@@ -807,7 +825,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>16</v>
@@ -836,7 +854,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>17</v>
@@ -865,7 +883,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>18</v>
@@ -893,8 +911,8 @@
       <c r="A14" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="11">
         <f>SUM(D5:D13)</f>
         <v>2690</v>

</xml_diff>